<commit_message>
updated asset tags levels
</commit_message>
<xml_diff>
--- a/asset_tags_list.xlsx
+++ b/asset_tags_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parvathykrishnank/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parvathykrishnank/Documents/GitHub/CCS RTD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BAD747-D9DA-8447-AEF6-C4AAC11D3F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5095A13-EABA-CE4E-92CD-53D8F8B1F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1500" windowWidth="26840" windowHeight="15820" xr2:uid="{F382DC95-34AF-B545-84A3-81E5EFC974E4}"/>
   </bookViews>
@@ -36,114 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Hard Investments (CAPEX)</t>
-  </si>
-  <si>
-    <t>Urban Roads</t>
-  </si>
-  <si>
-    <t>Highways</t>
-  </si>
-  <si>
-    <t>Rural Roads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRT stations </t>
-  </si>
-  <si>
-    <t>Buses stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridges </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Railway lines </t>
-  </si>
-  <si>
-    <t>Railway stations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trains stock </t>
-  </si>
-  <si>
-    <t>Floating Docks</t>
-  </si>
-  <si>
-    <t>Ferry Infrastructure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Airport Runways </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marine Navigation Equipment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Treatment Facility </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water supply </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solid waste treatment facilities </t>
-  </si>
-  <si>
-    <t>Transfer stations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste collection trucks stock </t>
-  </si>
-  <si>
-    <t>Bins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Landfills </t>
-  </si>
-  <si>
-    <t>Drainage (pipes, culverts)</t>
-  </si>
-  <si>
-    <t>Transmission Infrastructure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distribution Infrastructure </t>
-  </si>
-  <si>
-    <t>Mini Grids</t>
-  </si>
-  <si>
-    <t>Solar Panels</t>
-  </si>
-  <si>
-    <t>Buildings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afforestation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food storage facilities </t>
-  </si>
-  <si>
-    <t>Land rehabilitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSA trainings and capacity building </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partnership development /Access to finance </t>
-  </si>
-  <si>
-    <t>Cash transfer programs</t>
-  </si>
-  <si>
-    <t>Value chain development</t>
-  </si>
-  <si>
-    <t>Veterinary and phytosanitary services</t>
-  </si>
-  <si>
-    <t>Irrigation infrastructure</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Asset List Level 1</t>
+  </si>
+  <si>
+    <t>Aviation</t>
+  </si>
+  <si>
+    <t>Bridges</t>
+  </si>
+  <si>
+    <t>Broadband</t>
+  </si>
+  <si>
+    <t>Dams</t>
+  </si>
+  <si>
+    <t>Drinking Water</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Hazardous Waste</t>
+  </si>
+  <si>
+    <t>Inland Waterways</t>
+  </si>
+  <si>
+    <t>Ports</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>Roads</t>
+  </si>
+  <si>
+    <t>Schools</t>
+  </si>
+  <si>
+    <t>Solid Waste</t>
+  </si>
+  <si>
+    <t>Stormwater</t>
+  </si>
+  <si>
+    <t>Transit</t>
+  </si>
+  <si>
+    <t>Waste Water</t>
   </si>
 </sst>
 </file>
@@ -205,10 +148,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800858BF-E020-D242-A216-A56542AB79FF}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A36"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,101 +543,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated list asset tags
</commit_message>
<xml_diff>
--- a/asset_tags_list.xlsx
+++ b/asset_tags_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parvathykrishnank/Documents/GitHub/CCS RTD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5095A13-EABA-CE4E-92CD-53D8F8B1F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86B637-FF48-7547-8FEC-3378521B7B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1500" windowWidth="26840" windowHeight="15820" xr2:uid="{F382DC95-34AF-B545-84A3-81E5EFC974E4}"/>
+    <workbookView xWindow="480" yWindow="3480" windowWidth="26840" windowHeight="15820" xr2:uid="{F382DC95-34AF-B545-84A3-81E5EFC974E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>